<commit_message>
Added the latest changes
</commit_message>
<xml_diff>
--- a/src/test/resources/TeacherDetails.xlsx
+++ b/src/test/resources/TeacherDetails.xlsx
@@ -5,15 +5,14 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eclipse_Oxygen\schooltestLocal\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Github\SchoolMgmt\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14835" windowHeight="6075"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>Code</t>
   </si>
@@ -141,16 +140,13 @@
     <t>Branch</t>
   </si>
   <si>
-    <t>Andheri</t>
-  </si>
-  <si>
-    <t>123</t>
+    <t>123,Mumbai Branch</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -477,59 +473,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.140625" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:U2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>